<commit_message>
He pt bac nhat 3 an
</commit_message>
<xml_diff>
--- a/TH1_Nhom6_Unit_Testcase.xlsx
+++ b/TH1_Nhom6_Unit_Testcase.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Giao trinh\Chat luong va Kiem thu phan mem\Thuc hanh\Bai tap thuc hanh\Thuc hanh D14\TH1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TAI LIEU LAP TRINH\TDMU\Nam 4\Chat luong &amp; kiem thu phan mem\Thuc hanh\TH1\KiemThuPhanMem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E63DBAB-5529-4799-A12C-51EA16051DC1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16095" windowHeight="7440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16092" windowHeight="7440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ham 1" sheetId="1" r:id="rId1"/>
     <sheet name="PTB2" sheetId="2" r:id="rId2"/>
+    <sheet name="HPT3An" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Hàm</t>
   </si>
@@ -119,12 +121,67 @@
   </si>
   <si>
     <t>TC_PTB2_02</t>
+  </si>
+  <si>
+    <t>TC_HPT3A_01</t>
+  </si>
+  <si>
+    <t>TC_HPT3A_02</t>
+  </si>
+  <si>
+    <t>TC_HPT3A_03</t>
+  </si>
+  <si>
+    <t>Nhập vào a1=0, b1=0, c1=0, d1=0, a2=0, b2=0, c2=0, d2=0, a3=0, b3=0, c3=0, d3=0</t>
+  </si>
+  <si>
+    <t>Nhập vào a1=0, b1=0, c1=0, d1=1, a2=0, b2=0, c2=0, d2=0, a3=0, b3=0, c3=0, d3=0</t>
+  </si>
+  <si>
+    <t>Nhập vào a1=1, b1=1, c1=1, d1=6, a2=1, b2=-1, c2=1, d2=2, a3=1, b3=1, c3=-1, d3=0</t>
+  </si>
+  <si>
+    <t>Thông báo "Hệ phương trình có vô số nghiệm"</t>
+  </si>
+  <si>
+    <t>Hệ phương trình có vô số nghiệm</t>
+  </si>
+  <si>
+    <t>Thông báo "Hệ phương trình vô nghiệm"</t>
+  </si>
+  <si>
+    <t>Kiểm tra hệ phương trình vô số nghiệm</t>
+  </si>
+  <si>
+    <t>Kiểm tra hệ phương trình vô nghiệm</t>
+  </si>
+  <si>
+    <t>Kiểm tra hệ phương trình có một nghiệm</t>
+  </si>
+  <si>
+    <t>Hệ phương trình vô nghiệm</t>
+  </si>
+  <si>
+    <t>Message:   Expected string length 25 but was 28. Strings differ at index 19.
+  Expected: "Hệ phương trình vô nghiệm"
+  But was:  "Hệ phương trình vô số nghiệm"
+  ------------------------------^</t>
+  </si>
+  <si>
+    <t>Message:   Expected string length 27 but was 25. Strings differ at index 16.
+  Expected: "Hệ phương trình có 1 nghiệm"
+  But was:  "Hệ phương trình vô nghiệm"
+  ---------------------------^</t>
+  </si>
+  <si>
+    <t>Thông báo "Hệ phương trình có 1 nghiệm"
+Kết quả X=1, Y=2, Z=3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -205,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -238,6 +295,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,6 +401,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -367,6 +453,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -542,26 +645,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -574,7 +677,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -585,7 +688,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -608,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -631,7 +734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -642,7 +745,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -651,7 +754,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -660,7 +763,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -669,7 +772,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -678,7 +781,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -687,7 +790,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -704,7 +807,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -715,26 +818,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -747,7 +850,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -758,7 +861,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -781,7 +884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -804,7 +907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -827,7 +930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -848,7 +951,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -857,7 +960,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -866,7 +969,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -875,7 +978,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -884,7 +987,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -903,4 +1006,207 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349AF9C3-6409-42CC-9D3F-BE19C3871246}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="70" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="15" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="16" customFormat="1" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>